<commit_message>
update create trans to v2.1
</commit_message>
<xml_diff>
--- a/prepare_trans/excel_format/0_0.xlsx
+++ b/prepare_trans/excel_format/0_0.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -65,22 +65,16 @@
     <t>Angle</t>
   </si>
   <si>
-    <t>he_palaeo_0</t>
-  </si>
-  <si>
-    <t>he_palaeo_1</t>
-  </si>
-  <si>
-    <t>he_lexical_0</t>
-  </si>
-  <si>
-    <t>he_lexical_1</t>
-  </si>
-  <si>
-    <t>he_morphsyn_0</t>
-  </si>
-  <si>
-    <t>he_morphsyn_1</t>
+    <t>he_human_0</t>
+  </si>
+  <si>
+    <t>he_human_1</t>
+  </si>
+  <si>
+    <t>he_human_2</t>
+  </si>
+  <si>
+    <t>he_human_3</t>
   </si>
   <si>
     <t>line_id</t>
@@ -499,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -508,7 +502,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,14 +578,8 @@
       <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
+    </row>
+    <row r="2" spans="1:25">
       <c r="C2">
         <f>SIGNs!A2</f>
         <v>0</v>
@@ -600,7 +588,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:25">
       <c r="C3">
         <f>SIGNs!A3</f>
         <v>0</v>
@@ -609,7 +597,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:25">
       <c r="C4">
         <f>SIGNs!A4</f>
         <v>0</v>
@@ -618,7 +606,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:25">
       <c r="C5">
         <f>SIGNs!A5</f>
         <v>0</v>
@@ -627,7 +615,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:25">
       <c r="C6">
         <f>SIGNs!A6</f>
         <v>0</v>
@@ -636,7 +624,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:25">
       <c r="C7">
         <f>SIGNs!A7</f>
         <v>0</v>
@@ -645,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:25">
       <c r="C8">
         <f>SIGNs!A8</f>
         <v>0</v>
@@ -655,7 +643,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="105">
+  <dataValidations count="91">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
       <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
     </dataValidation>
@@ -674,15 +662,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1">
       <formula1>"certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
@@ -693,12 +681,6 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
@@ -719,15 +701,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2">
       <formula1>"certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
@@ -738,12 +720,6 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
@@ -764,15 +740,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3">
       <formula1>"certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
@@ -783,12 +759,6 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4">
@@ -809,15 +779,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4">
       <formula1>"certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W4">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X4">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y4">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z4">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
@@ -828,12 +798,6 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5">
@@ -854,15 +818,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5">
       <formula1>"certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W5">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y5">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z5">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
@@ -873,12 +837,6 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6">
@@ -899,15 +857,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6">
       <formula1>"certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V6">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W6">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X6">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q6">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
@@ -918,12 +876,6 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T6">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U6">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V6">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7">
@@ -944,15 +896,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7">
       <formula1>"certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7">
+      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z7">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
@@ -963,12 +915,6 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
   </dataValidations>
@@ -992,55 +938,55 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1048,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>546</v>
@@ -1098,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>1040</v>
@@ -1148,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>1232</v>
@@ -1198,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>735</v>
@@ -1248,7 +1194,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>1848</v>
@@ -1298,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7">
         <v>1911</v>
@@ -1348,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>3808</v>

</xml_diff>

<commit_message>
Updating Trans specs and Frag 1 a
</commit_message>
<xml_diff>
--- a/prepare_trans/excel_format/0_0.xlsx
+++ b/prepare_trans/excel_format/0_0.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="CHARs" sheetId="1" r:id="rId1"/>
     <sheet name="SIGNs" sheetId="2" r:id="rId2"/>
+    <sheet name="Sub_Frags" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -141,6 +142,12 @@
   </si>
   <si>
     <t>Solidity</t>
+  </si>
+  <si>
+    <t>frag_id</t>
+  </si>
+  <si>
+    <t>iaa_img_id</t>
   </si>
   <si>
     <t>42372_7.tif:0091-0415</t>
@@ -645,22 +652,22 @@
   </sheetData>
   <dataValidations count="91">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
+      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1">
-      <formula1>"False,True,relevant_w,relevant_h"</formula1>
+      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1">
-      <formula1>"certain,probable_letter,possible_letter"</formula1>
+      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
@@ -684,22 +691,22 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
+      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
-      <formula1>"False,True,relevant_w,relevant_h"</formula1>
+      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2">
-      <formula1>"certain,probable_letter,possible_letter"</formula1>
+      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
@@ -723,22 +730,22 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
+      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3">
-      <formula1>"False,True,relevant_w,relevant_h"</formula1>
+      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3">
-      <formula1>"certain,probable_letter,possible_letter"</formula1>
+      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
@@ -762,22 +769,22 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
+      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4">
-      <formula1>"False,True,relevant_w,relevant_h"</formula1>
+      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4">
-      <formula1>"certain,probable_letter,possible_letter"</formula1>
+      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
@@ -801,22 +808,22 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
+      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5">
-      <formula1>"False,True,relevant_w,relevant_h"</formula1>
+      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5">
-      <formula1>"certain,probable_letter,possible_letter"</formula1>
+      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
@@ -840,22 +847,22 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
+      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6">
-      <formula1>"False,True,relevant_w,relevant_h"</formula1>
+      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6">
-      <formula1>"certain,probable_letter,possible_letter"</formula1>
+      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V6">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
@@ -879,22 +886,22 @@
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased"</formula1>
+      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7">
-      <formula1>"False,True,relevant_w,relevant_h"</formula1>
+      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7">
-      <formula1>"True,False"</formula1>
+      <formula1>"null,True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7">
-      <formula1>"certain,probable_letter,possible_letter"</formula1>
+      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
@@ -994,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <v>546</v>
@@ -1044,7 +1051,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3">
         <v>1040</v>
@@ -1094,7 +1101,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <v>1232</v>
@@ -1144,7 +1151,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>735</v>
@@ -1194,7 +1201,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>1848</v>
@@ -1244,7 +1251,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>1911</v>
@@ -1294,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>3808</v>
@@ -1337,6 +1344,72 @@
       </c>
       <c r="R8">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>